<commit_message>
DAC Outputs scale correction
</commit_message>
<xml_diff>
--- a/hard/v0-CPU/CPU - PLsi_v0_estimated_cost.xlsx
+++ b/hard/v0-CPU/CPU - PLsi_v0_estimated_cost.xlsx
@@ -85,25 +85,7 @@
     <t xml:space="preserve">CPU</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Cambria"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.aliexpress.com/item/32959541446.html?spm=a2g0o.productlist.0.0.599c6fcaL6u7Ra&amp;algo_pvid=dcdac20a-031c-4cab-8970-70d47ca621fa&amp;algo_expid=dcdac20a-031c-4cab-8970-70d47ca621fa-1&amp;btsid=0bb0624316142121230811756e3b3c&amp;ws_ab_test=searchweb0_0,searchweb201602_,searchweb201603</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_</t>
-    </r>
+    <t xml:space="preserve">https://www.aliexpress.com/item/32959541446.html?spm=a2g0o.productlist.0.0.599c6fcaL6u7Ra&amp;algo_pvid=dcdac20a-031c-4cab-8970-70d47ca621fa&amp;algo_expid=dcdac20a-031c-4cab-8970-70d47ca621fa-1&amp;btsid=0bb0624316142121230811756e3b3c&amp;ws_ab_test=searchweb0_0,searchweb201602_,searchweb201603_</t>
   </si>
   <si>
     <t xml:space="preserve">digital outputs</t>
@@ -573,16 +555,17 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="11:11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.07"/>
   </cols>
   <sheetData>
@@ -688,7 +671,7 @@
         <v>17</v>
       </c>
       <c r="L5" s="13" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M5" s="14" t="s">
         <v>18</v>
@@ -731,7 +714,7 @@
         <v>22</v>
       </c>
       <c r="L6" s="13" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M6" s="14" t="s">
         <v>23</v>
@@ -775,7 +758,7 @@
         <v>27</v>
       </c>
       <c r="L7" s="13" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M7" s="14" t="s">
         <v>28</v>
@@ -819,7 +802,7 @@
         <v>31</v>
       </c>
       <c r="L8" s="13" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M8" s="14" t="s">
         <v>28</v>
@@ -890,11 +873,11 @@
       </c>
       <c r="F10" s="9" t="n">
         <f aca="false">L5+L6</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G10" s="9" t="n">
         <f aca="false">E10*F10</f>
-        <v>0.0532</v>
+        <v>0.07448</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>37</v>
@@ -936,11 +919,11 @@
       </c>
       <c r="F11" s="9" t="n">
         <f aca="false">L6</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G11" s="9" t="n">
         <f aca="false">E11*F11</f>
-        <v>1.0936</v>
+        <v>1.6404</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>22</v>
@@ -1007,11 +990,11 @@
       </c>
       <c r="F13" s="9" t="n">
         <f aca="false">L6</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G13" s="9" t="n">
         <f aca="false">E13*F13</f>
-        <v>0.0384</v>
+        <v>0.0576</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>44</v>
@@ -1043,11 +1026,11 @@
       </c>
       <c r="F14" s="9" t="n">
         <f aca="false">L5</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G14" s="9" t="n">
         <f aca="false">E14*F14</f>
-        <v>0.1644</v>
+        <v>0.2192</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>17</v>
@@ -1079,11 +1062,11 @@
       </c>
       <c r="F15" s="9" t="n">
         <f aca="false">L5</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G15" s="9" t="n">
         <f aca="false">E15*F15</f>
-        <v>0.078</v>
+        <v>0.104</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>17</v>
@@ -1115,11 +1098,11 @@
       </c>
       <c r="F16" s="9" t="n">
         <f aca="false">L5</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G16" s="9" t="n">
         <f aca="false">E16*F16</f>
-        <v>0.0576</v>
+        <v>0.0768</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>17</v>
@@ -1151,11 +1134,11 @@
       </c>
       <c r="F17" s="9" t="n">
         <f aca="false">L5</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G17" s="9" t="n">
         <f aca="false">E17*F17</f>
-        <v>0.1056</v>
+        <v>0.1408</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>17</v>
@@ -1187,11 +1170,11 @@
       </c>
       <c r="F18" s="9" t="n">
         <f aca="false">L5+L7*3+L8</f>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G18" s="9" t="n">
         <f aca="false">E18*F18</f>
-        <v>0.1344</v>
+        <v>0.0768</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>17</v>
@@ -1223,11 +1206,11 @@
       </c>
       <c r="F19" s="9" t="n">
         <f aca="false">$L$8/2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" s="9" t="n">
         <f aca="false">E19*F19</f>
-        <v>3.344</v>
+        <v>0</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>55</v>
@@ -1259,11 +1242,11 @@
       </c>
       <c r="F20" s="9" t="n">
         <f aca="false">$L$8</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G20" s="9" t="n">
         <f aca="false">E20*F20</f>
-        <v>0.0192</v>
+        <v>0</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>55</v>
@@ -1295,11 +1278,11 @@
       </c>
       <c r="F21" s="9" t="n">
         <f aca="false">$L$8</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G21" s="9" t="n">
         <f aca="false">E21*F21</f>
-        <v>0.0192</v>
+        <v>0</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>55</v>
@@ -1331,11 +1314,11 @@
       </c>
       <c r="F22" s="9" t="n">
         <f aca="false">$L$7*2</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G22" s="9" t="n">
         <f aca="false">E22*F22</f>
-        <v>0.0216</v>
+        <v>0</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>27</v>
@@ -1427,7 +1410,7 @@
       </c>
       <c r="G25" s="21" t="n">
         <f aca="false">SUM(G5:G24)</f>
-        <v>19.2740666666667</v>
+        <v>16.5349466666667</v>
       </c>
       <c r="I25" s="22"/>
     </row>
@@ -9238,7 +9221,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I5" r:id="rId1" display="https://www.aliexpress.com/item/32888213613.html?spm=a2g0s.9042311.0.0.27424c4d0qZ0bo"/>
-    <hyperlink ref="I6" r:id="rId2" display="https://www.aliexpress.com/item/32959541446.html?spm=a2g0o.productlist.0.0.599c6fcaL6u7Ra&amp;algo_pvid=dcdac20a-031c-4cab-8970-70d47ca621fa&amp;algo_expid=dcdac20a-031c-4cab-8970-70d47ca621fa-1&amp;btsid=0bb0624316142121230811756e3b3c&amp;ws_ab_test=searchweb0_0,searchweb201602_,searchweb201603"/>
+    <hyperlink ref="I6" r:id="rId2" display="https://www.aliexpress.com/item/32959541446.html?spm=a2g0o.productlist.0.0.599c6fcaL6u7Ra&amp;algo_pvid=dcdac20a-031c-4cab-8970-70d47ca621fa&amp;algo_expid=dcdac20a-031c-4cab-8970-70d47ca621fa-1&amp;btsid=0bb0624316142121230811756e3b3c&amp;ws_ab_test=searchweb0_0,searchweb201602_,searchweb201603_"/>
     <hyperlink ref="I7" r:id="rId3" display="https://www.aliexpress.com/item/32861400498.html?spm=a2g0s.9042311.0.0.27424c4d0qZ0bo"/>
     <hyperlink ref="I8" r:id="rId4" display="https://www.aliexpress.com/item/32864438850.html?spm=a2g0s.9042311.0.0.27424c4dtHH5qT"/>
     <hyperlink ref="I9" r:id="rId5" display="https://www.aliexpress.com/item/32812085542.html?spm=a2g0s.9042311.0.0.27424c4d0qZ0bo"/>

</xml_diff>